<commit_message>
NSMB - v3 movie file added
</commit_message>
<xml_diff>
--- a/trunk/NSMB/NSMB.xlsx
+++ b/trunk/NSMB/NSMB.xlsx
@@ -141,9 +141,6 @@
     <t>Place</t>
   </si>
   <si>
-    <t>V2</t>
-  </si>
-  <si>
     <t>Diff</t>
   </si>
   <si>
@@ -217,6 +214,9 @@
   </si>
   <si>
     <t>Level 5-3</t>
+  </si>
+  <si>
+    <t>V3</t>
   </si>
 </sst>
 </file>
@@ -273,7 +273,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -293,6 +293,26 @@
     <border>
       <left/>
       <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom style="double">
         <color indexed="64"/>
@@ -301,7 +321,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="double">
         <color indexed="64"/>
       </top>
@@ -312,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -340,14 +362,15 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -644,14 +667,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="13" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" style="18" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="18"/>
+    <col min="5" max="5" width="13" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickBot="1">
@@ -659,360 +683,360 @@
         <v>40</v>
       </c>
       <c r="B1" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" s="16" t="s">
-        <v>42</v>
-      </c>
       <c r="E1" s="16" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="17" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="13" customFormat="1" ht="19.5" thickTop="1">
+      <c r="A2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="B3">
+      <c r="A3" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="18">
         <v>355</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="18">
         <v>355</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="18">
         <f>IF(B3 &gt;  0,C3-B3, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B4">
+      <c r="A4" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="18">
         <v>517</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="18">
         <v>517</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="18">
         <f t="shared" ref="D4:D6" si="0">IF(B4 &gt;  0,C4-B4, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5">
+      <c r="A5" s="18" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="18">
         <v>2937</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="18">
         <v>2937</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B6">
-        <v>3133</v>
-      </c>
-      <c r="C6">
-        <v>3162</v>
-      </c>
-      <c r="D6">
+      <c r="A6" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="18">
+        <v>3128</v>
+      </c>
+      <c r="C6" s="18">
+        <v>3131</v>
+      </c>
+      <c r="D6" s="18">
         <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="17" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A7" s="20" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" s="13" customFormat="1" ht="19.5" thickTop="1">
+      <c r="A7" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="21">
+        <f>D6</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="13">
-        <f>D6</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
+      <c r="B8" s="19"/>
+      <c r="C8" s="19"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9">
+      <c r="A9" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="18">
         <v>3380</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="18">
         <v>3380</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="18">
         <f>IF(B9 &gt;  0,C9-B9, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="D10">
+      <c r="D10" s="18">
         <f t="shared" ref="D10:D19" si="1">IF(B10 &gt;  0,C10-B10, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="D11">
+      <c r="D11" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="D12">
+      <c r="D12" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B13">
+      <c r="A13" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="18">
         <v>4724</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="18">
         <v>4727</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="18">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="18">
         <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14">
+      <c r="A14" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="18">
         <v>5242</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="18">
         <v>5245</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="18">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:5">
-      <c r="A15" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B15" s="15">
+      <c r="A15" s="19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="19">
         <v>5832</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C15" s="19">
         <v>5835</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="18">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="E15" s="15"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="1:5">
-      <c r="A16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16">
+      <c r="A16" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="18">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:5">
-      <c r="A17" t="s">
-        <v>58</v>
-      </c>
-      <c r="B17">
+      <c r="A17" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="18">
         <v>6028</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="18">
         <f t="shared" si="1"/>
         <v>-6028</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18">
+      <c r="A18" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18" s="18">
         <v>8345</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="18">
         <v>8352</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="18">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="18">
         <v>359</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19">
+      <c r="A19" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="18">
         <v>8859</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="18">
         <v>8866</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="18">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" t="s">
+      <c r="A20" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="18">
+        <v>11169</v>
+      </c>
+      <c r="C21" s="18">
+        <v>11172</v>
+      </c>
+      <c r="E21" s="18">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" s="18">
+        <v>11349</v>
+      </c>
+      <c r="C22" s="18">
+        <v>11354</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="18" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" t="s">
+      <c r="B23" s="18">
+        <v>11870</v>
+      </c>
+      <c r="E23" s="18">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="18">
+        <v>12181</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="B21">
-        <v>11169</v>
-      </c>
-      <c r="C21">
-        <v>11172</v>
-      </c>
-      <c r="E21">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" t="s">
-        <v>61</v>
-      </c>
-      <c r="B22">
-        <v>11349</v>
-      </c>
-      <c r="C22">
-        <v>11354</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" t="s">
-        <v>60</v>
-      </c>
-      <c r="B23">
-        <v>11870</v>
-      </c>
-      <c r="E23">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" t="s">
+      <c r="B25" s="18">
+        <v>12695</v>
+      </c>
+      <c r="E25" s="18">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" s="18">
+        <v>14395</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="20"/>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="18">
+        <v>17101</v>
+      </c>
+      <c r="C30" s="18">
+        <v>365</v>
+      </c>
+      <c r="E30" s="18">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B24">
-        <v>12181</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" t="s">
-        <v>63</v>
-      </c>
-      <c r="B25">
-        <v>12695</v>
-      </c>
-      <c r="E25">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" t="s">
-        <v>64</v>
-      </c>
-      <c r="B26">
-        <v>14395</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="18"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" t="s">
+      <c r="B31" s="18">
+        <v>17615</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="20" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
-      <c r="A30" t="s">
+    <row r="34" spans="1:2">
+      <c r="A34" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B34" s="18">
+        <v>24271</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="B30">
-        <v>17101</v>
-      </c>
-      <c r="C30">
-        <v>365</v>
-      </c>
-      <c r="E30">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" t="s">
-        <v>47</v>
-      </c>
-      <c r="B31">
-        <v>17615</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="18" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" t="s">
-        <v>46</v>
-      </c>
-      <c r="B34">
-        <v>24271</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" t="s">
-        <v>47</v>
-      </c>
-      <c r="B35">
+      <c r="B35" s="18">
         <v>24786</v>
       </c>
     </row>

</xml_diff>

<commit_message>
NSMB - 1-1 completed 9 frames faster than my v2 attempt from some months ago.  All 9 frames come from a corner boosting technique.
</commit_message>
<xml_diff>
--- a/trunk/NSMB/NSMB.xlsx
+++ b/trunk/NSMB/NSMB.xlsx
@@ -363,14 +363,14 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -668,375 +668,349 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" style="18" customWidth="1"/>
-    <col min="2" max="4" width="9.140625" style="18"/>
-    <col min="5" max="5" width="13" style="18" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" style="16" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="16"/>
+    <col min="5" max="5" width="13" style="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5" thickBot="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="14" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="18">
+      <c r="B3" s="16">
         <v>355</v>
       </c>
-      <c r="C3" s="18">
+      <c r="C3" s="16">
         <v>355</v>
       </c>
-      <c r="D3" s="18">
+      <c r="D3" s="16">
         <f>IF(B3 &gt;  0,C3-B3, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="18">
+      <c r="B4" s="16">
         <v>517</v>
       </c>
-      <c r="C4" s="18">
+      <c r="C4" s="16">
         <v>517</v>
       </c>
-      <c r="D4" s="18">
+      <c r="D4" s="16">
         <f t="shared" ref="D4:D6" si="0">IF(B4 &gt;  0,C4-B4, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <v>2937</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="16">
         <v>2937</v>
       </c>
-      <c r="D5" s="18">
+      <c r="D5" s="16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="18">
+      <c r="B6" s="16">
         <v>3128</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="16">
         <v>3131</v>
       </c>
-      <c r="D6" s="18">
+      <c r="D6" s="16">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:5" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="21">
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="19">
         <f>D6</f>
         <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
+      <c r="B8" s="17"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="18">
+      <c r="B9" s="16">
         <v>3380</v>
       </c>
-      <c r="C9" s="18">
+      <c r="C9" s="16">
         <v>3380</v>
       </c>
-      <c r="D9" s="18">
+      <c r="D9" s="16">
         <f>IF(B9 &gt;  0,C9-B9, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
-      <c r="D10" s="18">
+      <c r="D10" s="16">
         <f t="shared" ref="D10:D19" si="1">IF(B10 &gt;  0,C10-B10, 0)</f>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="D11" s="18">
+      <c r="D11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="D12" s="18">
+      <c r="D12" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:5">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="18">
+      <c r="B13" s="16">
+        <v>4715</v>
+      </c>
+      <c r="C13" s="16">
         <v>4724</v>
       </c>
-      <c r="C13" s="18">
-        <v>4727</v>
-      </c>
-      <c r="D13" s="18">
+      <c r="D13" s="16">
         <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E13" s="18">
+        <v>9</v>
+      </c>
+      <c r="E13" s="16">
         <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:5">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="18">
-        <v>5242</v>
-      </c>
-      <c r="C14" s="18">
+      <c r="C14" s="16">
         <v>5245</v>
       </c>
-      <c r="D14" s="18">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15" s="19">
-        <v>5832</v>
-      </c>
-      <c r="C15" s="19">
-        <v>5835</v>
-      </c>
-      <c r="D15" s="18">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="E15" s="19"/>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="D16" s="18">
+      <c r="D14" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17">
+        <v>5835</v>
+      </c>
+      <c r="D15" s="16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="E15" s="17"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="16">
+        <v>6019</v>
+      </c>
+      <c r="C16" s="16">
+        <v>6028</v>
+      </c>
+      <c r="D16" s="16">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+    </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="18">
-        <v>6028</v>
-      </c>
-      <c r="D17" s="18">
+      <c r="D17" s="16">
         <f t="shared" si="1"/>
-        <v>-6028</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="18">
-        <v>8345</v>
-      </c>
-      <c r="C18" s="18">
+      <c r="C18" s="16">
         <v>8352</v>
       </c>
-      <c r="D18" s="18">
+      <c r="D18" s="16">
         <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="E18" s="18">
+        <v>0</v>
+      </c>
+      <c r="E18" s="16">
         <v>359</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B19" s="18">
-        <v>8859</v>
-      </c>
-      <c r="C19" s="18">
+      <c r="C19" s="16">
         <v>8866</v>
       </c>
-      <c r="D19" s="18">
+      <c r="D19" s="16">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="16" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="18">
-        <v>11169</v>
-      </c>
-      <c r="C21" s="18">
+      <c r="C21" s="16">
         <v>11172</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="16">
         <v>480</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B22" s="18">
-        <v>11349</v>
-      </c>
-      <c r="C22" s="18">
+      <c r="C22" s="16">
         <v>11354</v>
       </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="18">
-        <v>11870</v>
-      </c>
-      <c r="E23" s="18">
+      <c r="E23" s="16">
         <v>469</v>
       </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B24" s="18">
-        <v>12181</v>
-      </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="18">
-        <v>12695</v>
-      </c>
-      <c r="E25" s="18">
+      <c r="E25" s="16">
         <v>465</v>
       </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="18">
-        <v>14395</v>
-      </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="20"/>
+      <c r="A27" s="18"/>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="18" t="s">
+      <c r="A29" s="16" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="18" t="s">
+      <c r="A30" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="18">
+      <c r="B30" s="16">
         <v>17101</v>
       </c>
-      <c r="C30" s="18">
+      <c r="C30" s="16">
         <v>365</v>
       </c>
-      <c r="E30" s="18">
+      <c r="E30" s="16">
         <v>365</v>
       </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="18" t="s">
+      <c r="A31" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="18">
+      <c r="B31" s="16">
         <v>17615</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="20" t="s">
+      <c r="A33" s="18" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="34" spans="1:2">
-      <c r="A34" s="18" t="s">
+      <c r="A34" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B34" s="18">
+      <c r="B34" s="16">
         <v>24271</v>
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="18" t="s">
+      <c r="A35" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="18">
+      <c r="B35" s="16">
         <v>24786</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1-2 Complete.  1 faster in level due to corner boosting.  28 faster on the map due to better randomness.  38 ahead total.
</commit_message>
<xml_diff>
--- a/trunk/NSMB/NSMB.xlsx
+++ b/trunk/NSMB/NSMB.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="135" windowWidth="16080" windowHeight="7500"/>
   </bookViews>
   <sheets>
-    <sheet name="V2" sheetId="2" r:id="rId1"/>
+    <sheet name="V3" sheetId="2" r:id="rId1"/>
     <sheet name="V1" sheetId="1" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="66">
   <si>
     <t>1-1</t>
   </si>
@@ -177,9 +177,6 @@
     <t>First move</t>
   </si>
   <si>
-    <t>Level end</t>
-  </si>
-  <si>
     <t>Best</t>
   </si>
   <si>
@@ -189,12 +186,6 @@
     <t>enter 1-2</t>
   </si>
   <si>
-    <t>black screen</t>
-  </si>
-  <si>
-    <t>1-C</t>
-  </si>
-  <si>
     <t>Enter pipe BS</t>
   </si>
   <si>
@@ -217,6 +208,12 @@
   </si>
   <si>
     <t>V3</t>
+  </si>
+  <si>
+    <t>End 1-2</t>
+  </si>
+  <si>
+    <t>Enter 1-C</t>
   </si>
 </sst>
 </file>
@@ -668,7 +665,7 @@
   <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -683,10 +680,10 @@
         <v>40</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>41</v>
@@ -850,7 +847,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B15" s="17"/>
       <c r="C15" s="17">
@@ -864,7 +861,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B16" s="16">
         <v>6019</v>
@@ -879,48 +876,46 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="16" t="s">
-        <v>57</v>
+        <v>64</v>
+      </c>
+      <c r="B17" s="16">
+        <v>8849</v>
+      </c>
+      <c r="C17" s="16">
+        <v>8859</v>
       </c>
       <c r="D17" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="16" t="s">
-        <v>53</v>
+        <v>65</v>
+      </c>
+      <c r="B18" s="16">
+        <v>9865</v>
       </c>
       <c r="C18" s="16">
-        <v>8352</v>
+        <v>9903</v>
       </c>
       <c r="D18" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="E18" s="16">
         <v>359</v>
       </c>
     </row>
     <row r="19" spans="1:5">
-      <c r="A19" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" s="16">
-        <v>8866</v>
-      </c>
       <c r="D19" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="16" t="s">
-        <v>58</v>
-      </c>
-    </row>
     <row r="21" spans="1:5">
       <c r="A21" s="16" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C21" s="16">
         <v>11172</v>
@@ -931,7 +926,7 @@
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="16" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C22" s="16">
         <v>11354</v>
@@ -939,7 +934,7 @@
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="16" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="E23" s="16">
         <v>469</v>
@@ -952,7 +947,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="16" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E25" s="16">
         <v>465</v>
@@ -960,7 +955,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="16" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -968,7 +963,7 @@
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="16" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -995,7 +990,7 @@
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="18" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:2">

</xml_diff>

<commit_message>
NSMB - finished the vertical section of 1-C.  Improved it by 14 frames over my previous attempt and 8 frames over was0x's movie.
</commit_message>
<xml_diff>
--- a/trunk/NSMB/NSMB.xlsx
+++ b/trunk/NSMB/NSMB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
   <si>
     <t>1-1</t>
   </si>
@@ -171,36 +171,15 @@
     <t>Enter 1-1</t>
   </si>
   <si>
-    <t>Game time</t>
-  </si>
-  <si>
     <t>First move</t>
   </si>
   <si>
-    <t>Best</t>
-  </si>
-  <si>
     <t>map - first move</t>
   </si>
   <si>
     <t>enter 1-2</t>
   </si>
   <si>
-    <t>Enter pipe BS</t>
-  </si>
-  <si>
-    <t>Enter secret BS</t>
-  </si>
-  <si>
-    <t>Enter door BS</t>
-  </si>
-  <si>
-    <t>End level</t>
-  </si>
-  <si>
-    <t>1-C BS</t>
-  </si>
-  <si>
     <t>Level 5-1</t>
   </si>
   <si>
@@ -214,6 +193,30 @@
   </si>
   <si>
     <t>Enter 1-C</t>
+  </si>
+  <si>
+    <t>First jump</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>Was0x</t>
+  </si>
+  <si>
+    <t>3rd Jump</t>
+  </si>
+  <si>
+    <t>6th jump</t>
+  </si>
+  <si>
+    <t>Jump after block corridor</t>
+  </si>
+  <si>
+    <t>Next jump</t>
+  </si>
+  <si>
+    <t>Enter Door</t>
   </si>
 </sst>
 </file>
@@ -244,7 +247,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,8 +272,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -285,15 +294,6 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -316,22 +316,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -360,14 +349,17 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -662,46 +654,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E35"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27.7109375" style="16" customWidth="1"/>
     <col min="2" max="4" width="9.140625" style="16"/>
-    <col min="5" max="5" width="13" style="16" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="16"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="16.5" thickBot="1">
+    <row r="1" spans="1:6" ht="16.5" thickBot="1">
       <c r="A1" s="14" t="s">
         <v>40</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="E1" s="14" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="13" customFormat="1" ht="19.5" thickTop="1">
+      <c r="E1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="13" customFormat="1" ht="19.5" thickTop="1">
       <c r="A2" s="20" t="s">
         <v>44</v>
       </c>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="15" t="s">
         <v>47</v>
       </c>
@@ -716,7 +713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:6">
       <c r="A4" s="16" t="s">
         <v>48</v>
       </c>
@@ -731,7 +728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:6">
       <c r="A5" s="16" t="s">
         <v>49</v>
       </c>
@@ -746,7 +743,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" thickBot="1">
+    <row r="6" spans="1:6">
       <c r="A6" s="16" t="s">
         <v>50</v>
       </c>
@@ -761,30 +758,29 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A7" s="21" t="s">
+    <row r="7" spans="1:6" s="13" customFormat="1" ht="18.75">
+      <c r="A7" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="21"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="19">
-        <f>D6</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="17" t="s">
+      <c r="B7" s="22"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="17"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="24"/>
+      <c r="F8" s="23"/>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9" s="16" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="16">
         <v>3380</v>
@@ -797,225 +793,257 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:6">
+      <c r="A10" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B10" s="16">
+        <v>4715</v>
+      </c>
+      <c r="C10" s="16">
+        <v>4724</v>
+      </c>
       <c r="D10" s="16">
-        <f t="shared" ref="D10:D19" si="1">IF(B10 &gt;  0,C10-B10, 0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <f t="shared" ref="D10:D21" si="1">IF(B10 &gt;  0,C10-B10, 0)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="16">
+        <v>5245</v>
+      </c>
       <c r="D11" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:6">
+      <c r="A12" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17">
+        <v>5835</v>
+      </c>
       <c r="D12" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:6">
       <c r="A13" s="16" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B13" s="16">
-        <v>4715</v>
+        <v>6019</v>
       </c>
       <c r="C13" s="16">
-        <v>4724</v>
+        <v>6028</v>
       </c>
       <c r="D13" s="16">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="E13" s="16">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14" s="16" t="s">
-        <v>46</v>
+        <v>57</v>
+      </c>
+      <c r="B14" s="16">
+        <v>8849</v>
       </c>
       <c r="C14" s="16">
-        <v>5245</v>
+        <v>8859</v>
       </c>
       <c r="D14" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17">
-        <v>5835</v>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B15" s="16">
+        <v>9865</v>
+      </c>
+      <c r="C15" s="16">
+        <v>9903</v>
       </c>
       <c r="D15" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E15" s="17"/>
-    </row>
-    <row r="16" spans="1:5">
+        <v>38</v>
+      </c>
+      <c r="E15">
+        <v>9880</v>
+      </c>
+      <c r="F15" s="16">
+        <f>IF(B15 &gt;  0,E15-B15, 0)</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16" s="16" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B16" s="16">
-        <v>6019</v>
+        <v>10110</v>
       </c>
       <c r="C16" s="16">
-        <v>6028</v>
+        <v>10150</v>
       </c>
       <c r="D16" s="16">
         <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5">
+        <v>40</v>
+      </c>
+      <c r="E16">
+        <v>10128</v>
+      </c>
+      <c r="F16" s="16">
+        <f>IF(B16 &gt;  0,E16-B16, 0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B17" s="16">
-        <v>8849</v>
+        <v>10165</v>
       </c>
       <c r="C17" s="16">
-        <v>8859</v>
+        <v>10208</v>
       </c>
       <c r="D17" s="16">
         <f t="shared" si="1"/>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5">
+        <v>43</v>
+      </c>
+      <c r="E17">
+        <v>10186</v>
+      </c>
+      <c r="F17" s="16">
+        <f>IF(B17 &gt;  0,E17-B17, 0)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="16">
-        <v>9865</v>
-      </c>
-      <c r="C18" s="16">
-        <v>9903</v>
-      </c>
-      <c r="D18" s="16">
-        <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="E18" s="16">
-        <v>359</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
+        <v>63</v>
+      </c>
+      <c r="E18">
+        <v>10254</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B19" s="16">
+        <v>10733</v>
+      </c>
+      <c r="C19" s="16">
+        <v>10777</v>
+      </c>
       <c r="D19" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
+        <v>44</v>
+      </c>
+      <c r="E19">
+        <v>10746</v>
+      </c>
+      <c r="F19" s="16">
+        <f>IF(B19 &gt;  0,E19-B19, 0)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="E20">
+        <v>10769</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21" s="16" t="s">
-        <v>58</v>
+        <v>66</v>
+      </c>
+      <c r="B21" s="16">
+        <v>11117</v>
       </c>
       <c r="C21" s="16">
-        <v>11172</v>
-      </c>
-      <c r="E21" s="16">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="A22" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C22" s="16">
-        <v>11354</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="E23" s="16">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="16" t="s">
+        <v>11169</v>
+      </c>
+      <c r="D21" s="16">
+        <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="E21">
+        <v>11144</v>
+      </c>
+      <c r="F21" s="16">
+        <f>IF(B21 &gt;  0,E21-B21, 0)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="18"/>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" s="16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="16" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="E25" s="16">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="16" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="18"/>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="16" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="16" t="s">
+      <c r="B27" s="16">
+        <v>17101</v>
+      </c>
+      <c r="C27" s="16">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B28" s="16">
+        <v>17615</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="16">
-        <v>17101</v>
-      </c>
-      <c r="C30" s="16">
-        <v>365</v>
-      </c>
-      <c r="E30" s="16">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="16" t="s">
+      <c r="B31" s="16">
+        <v>24271</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="16">
-        <v>17615</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B34" s="16">
-        <v>24271</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="16">
+      <c r="B32" s="16">
         <v>24786</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A2:E2"/>
-    <mergeCell ref="A7:D7"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A7:F7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967294" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
NSMB - 1-F done, 88 ahead of my previous wip, 18 ahead of Was0x.  I still need to test manipulating the map movements.
</commit_message>
<xml_diff>
--- a/trunk/NSMB/NSMB.xlsx
+++ b/trunk/NSMB/NSMB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
   <si>
     <t>1-1</t>
   </si>
@@ -180,12 +180,6 @@
     <t>enter 1-2</t>
   </si>
   <si>
-    <t>Level 5-1</t>
-  </si>
-  <si>
-    <t>Level 5-3</t>
-  </si>
-  <si>
     <t>V3</t>
   </si>
   <si>
@@ -217,6 +211,39 @@
   </si>
   <si>
     <t>Enter Door</t>
+  </si>
+  <si>
+    <t>Enter secret room</t>
+  </si>
+  <si>
+    <t>Break first brick</t>
+  </si>
+  <si>
+    <t>Break 2nd brick</t>
+  </si>
+  <si>
+    <t>Break 3rd brick</t>
+  </si>
+  <si>
+    <t>Checkpoint 954</t>
+  </si>
+  <si>
+    <t>Checkpoint 987</t>
+  </si>
+  <si>
+    <t>Checkpoint 1063</t>
+  </si>
+  <si>
+    <t>Enter Pipe</t>
+  </si>
+  <si>
+    <t>Level End</t>
+  </si>
+  <si>
+    <t>Map 1st move</t>
+  </si>
+  <si>
+    <t>Enter 1-F</t>
   </si>
 </sst>
 </file>
@@ -355,11 +382,11 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,11 +681,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -673,30 +700,30 @@
         <v>40</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C1" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D1" s="14" t="s">
         <v>41</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F1" s="19" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="15" t="s">
@@ -759,24 +786,24 @@
       </c>
     </row>
     <row r="7" spans="1:6" s="13" customFormat="1" ht="18.75">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="23"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="16" t="s">
@@ -804,7 +831,7 @@
         <v>4724</v>
       </c>
       <c r="D10" s="16">
-        <f t="shared" ref="D10:D21" si="1">IF(B10 &gt;  0,C10-B10, 0)</f>
+        <f t="shared" ref="D10:D33" si="1">IF(B10 &gt;  0,C10-B10, 0)</f>
         <v>9</v>
       </c>
     </row>
@@ -850,7 +877,7 @@
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="16" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B14" s="16">
         <v>8849</v>
@@ -865,7 +892,7 @@
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="16" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B15" s="16">
         <v>9865</v>
@@ -887,7 +914,7 @@
     </row>
     <row r="16" spans="1:6">
       <c r="A16" s="16" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B16" s="16">
         <v>10110</v>
@@ -909,7 +936,7 @@
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B17" s="16">
         <v>10165</v>
@@ -931,7 +958,7 @@
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E18">
         <v>10254</v>
@@ -939,7 +966,7 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B19" s="16">
         <v>10733</v>
@@ -961,7 +988,7 @@
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="16" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E20">
         <v>10769</v>
@@ -969,7 +996,7 @@
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B21" s="16">
         <v>11117</v>
@@ -989,52 +1016,261 @@
         <v>27</v>
       </c>
     </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" s="16">
+        <v>11298</v>
+      </c>
+      <c r="C22" s="16">
+        <v>11349</v>
+      </c>
+      <c r="D22" s="16">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="E22">
+        <v>11325</v>
+      </c>
+      <c r="F22" s="16">
+        <f>IF(B22 &gt;  0,E22-B22, 0)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
+      <c r="A23" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="16">
+        <v>11439</v>
+      </c>
+      <c r="C23" s="16">
+        <v>11490</v>
+      </c>
+      <c r="D23" s="16">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="E23">
+        <v>11466</v>
+      </c>
+      <c r="F23" s="16">
+        <f>IF(B23 &gt;  0,E23-B23, 0)</f>
+        <v>27</v>
+      </c>
+    </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="18"/>
+      <c r="A24" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="B24" s="16">
+        <v>11491</v>
+      </c>
+      <c r="C24" s="16">
+        <v>11542</v>
+      </c>
+      <c r="D24" s="16">
+        <f t="shared" si="1"/>
+        <v>51</v>
+      </c>
+      <c r="E24">
+        <v>11517</v>
+      </c>
+      <c r="F24" s="16">
+        <f>IF(B24 &gt;  0,E24-B24, 0)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B25" s="16">
+        <v>11552</v>
+      </c>
+      <c r="C25" s="16">
+        <v>11606</v>
+      </c>
+      <c r="D25" s="16">
+        <f t="shared" si="1"/>
+        <v>54</v>
+      </c>
+      <c r="E25">
+        <v>11577</v>
+      </c>
+      <c r="F25" s="16">
+        <f>IF(B25 &gt;  0,E25-B25, 0)</f>
+        <v>25</v>
+      </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="16" t="s">
-        <v>54</v>
+        <v>69</v>
+      </c>
+      <c r="B26" s="16">
+        <v>11616</v>
+      </c>
+      <c r="C26" s="16">
+        <v>11672</v>
+      </c>
+      <c r="D26" s="16">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="E26">
+        <v>11644</v>
+      </c>
+      <c r="F26" s="16">
+        <f>IF(B26 &gt;  0,E26-B26, 0)</f>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="16" t="s">
-        <v>45</v>
+        <v>70</v>
       </c>
       <c r="B27" s="16">
-        <v>17101</v>
+        <v>11626</v>
       </c>
       <c r="C27" s="16">
-        <v>365</v>
+        <v>11682</v>
+      </c>
+      <c r="D27" s="16">
+        <f t="shared" si="1"/>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="16" t="s">
-        <v>46</v>
+        <v>71</v>
       </c>
       <c r="B28" s="16">
-        <v>17615</v>
+        <v>11652</v>
+      </c>
+      <c r="C28" s="16">
+        <v>11708</v>
+      </c>
+      <c r="D28" s="16">
+        <f t="shared" si="1"/>
+        <v>56</v>
+      </c>
+      <c r="E28">
+        <v>11680</v>
+      </c>
+      <c r="F28" s="16">
+        <f>IF(B28 &gt;  0,E28-B28, 0)</f>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B29" s="16">
+        <v>11810</v>
+      </c>
+      <c r="C29" s="16">
+        <v>11870</v>
+      </c>
+      <c r="D29" s="16">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E29">
+        <v>11839</v>
+      </c>
+      <c r="F29" s="16">
+        <f>IF(B29 &gt;  0,E29-B29, 0)</f>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:6">
       <c r="A30" s="18" t="s">
-        <v>55</v>
+        <v>45</v>
+      </c>
+      <c r="B30" s="16">
+        <v>12121</v>
+      </c>
+      <c r="C30" s="16">
+        <v>12181</v>
+      </c>
+      <c r="D30" s="16">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E30">
+        <v>12150</v>
+      </c>
+      <c r="F30" s="16">
+        <f>IF(B30 &gt;  0,E30-B30, 0)</f>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="16" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="B31" s="16">
-        <v>24271</v>
+        <v>12635</v>
+      </c>
+      <c r="C31" s="16">
+        <v>12695</v>
+      </c>
+      <c r="D31" s="16">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E31">
+        <v>12664</v>
+      </c>
+      <c r="F31" s="16">
+        <f>IF(B31 &gt;  0,E31-B31, 0)</f>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="16" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="B32" s="16">
-        <v>24786</v>
+        <v>13099</v>
+      </c>
+      <c r="C32" s="16">
+        <v>13187</v>
+      </c>
+      <c r="D32" s="16">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="E32">
+        <v>13117</v>
+      </c>
+      <c r="F32" s="16">
+        <f>IF(B32 &gt;  0,E32-B32, 0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="16">
+        <v>13343</v>
+      </c>
+      <c r="C33" s="16">
+        <v>13431</v>
+      </c>
+      <c r="D33" s="16">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="E33">
+        <v>13361</v>
+      </c>
+      <c r="F33" s="16">
+        <f>IF(B33 &gt;  0,E33-B33, 0)</f>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
5-1 done.  240 frames faster than my v2 wip.  16 faster than was0x's wip.  Most of the improvement comes from map movement manipulation.
</commit_message>
<xml_diff>
--- a/trunk/NSMB/NSMB.xlsx
+++ b/trunk/NSMB/NSMB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
   <si>
     <t>1-1</t>
   </si>
@@ -244,6 +244,30 @@
   </si>
   <si>
     <t>Enter 1-F</t>
+  </si>
+  <si>
+    <t>1-C End</t>
+  </si>
+  <si>
+    <t>World 5</t>
+  </si>
+  <si>
+    <t>Level 5-1</t>
+  </si>
+  <si>
+    <t>Enter 5-1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Level 1-2</t>
+  </si>
+  <si>
+    <t>Level 1-F</t>
+  </si>
+  <si>
+    <t>Checkpoint 12288</t>
+  </si>
+  <si>
+    <t>End Level</t>
   </si>
 </sst>
 </file>
@@ -274,7 +298,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -302,6 +326,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -347,7 +383,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -384,9 +420,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="0" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -681,11 +722,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -716,14 +757,14 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="13" customFormat="1" ht="19.5" thickTop="1">
-      <c r="A2" s="22" t="s">
+      <c r="A2" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="15" t="s">
@@ -786,14 +827,14 @@
       </c>
     </row>
     <row r="7" spans="1:6" s="13" customFormat="1" ht="18.75">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="20" t="s">
@@ -831,7 +872,7 @@
         <v>4724</v>
       </c>
       <c r="D10" s="16">
-        <f t="shared" ref="D10:D33" si="1">IF(B10 &gt;  0,C10-B10, 0)</f>
+        <f t="shared" ref="D10:D36" si="1">IF(B10 &gt;  0,C10-B10, 0)</f>
         <v>9</v>
       </c>
     </row>
@@ -861,422 +902,642 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="16" t="s">
-        <v>53</v>
-      </c>
-      <c r="B13" s="16">
-        <v>6019</v>
-      </c>
-      <c r="C13" s="16">
-        <v>6028</v>
-      </c>
-      <c r="D13" s="16">
-        <f t="shared" si="1"/>
-        <v>9</v>
-      </c>
+      <c r="A13" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" s="16" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B14" s="16">
-        <v>8849</v>
+        <v>6019</v>
       </c>
       <c r="C14" s="16">
-        <v>8859</v>
+        <v>6028</v>
       </c>
       <c r="D14" s="16">
         <f t="shared" si="1"/>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" s="16" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B15" s="16">
-        <v>9865</v>
+        <v>8849</v>
       </c>
       <c r="C15" s="16">
-        <v>9903</v>
+        <v>8859</v>
       </c>
       <c r="D15" s="16">
         <f t="shared" si="1"/>
-        <v>38</v>
-      </c>
-      <c r="E15">
-        <v>9880</v>
-      </c>
-      <c r="F15" s="16">
-        <f>IF(B15 &gt;  0,E15-B15, 0)</f>
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="B16" s="16">
-        <v>10110</v>
-      </c>
-      <c r="C16" s="16">
-        <v>10150</v>
-      </c>
-      <c r="D16" s="16">
-        <f t="shared" si="1"/>
-        <v>40</v>
-      </c>
-      <c r="E16">
-        <v>10128</v>
-      </c>
-      <c r="F16" s="16">
-        <f>IF(B16 &gt;  0,E16-B16, 0)</f>
-        <v>18</v>
-      </c>
+      <c r="A16" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="20"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" spans="1:6">
       <c r="A17" s="16" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="B17" s="16">
-        <v>10165</v>
+        <v>9865</v>
       </c>
       <c r="C17" s="16">
-        <v>10208</v>
+        <v>9903</v>
       </c>
       <c r="D17" s="16">
         <f t="shared" si="1"/>
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="E17">
-        <v>10186</v>
+        <v>9880</v>
       </c>
       <c r="F17" s="16">
         <f>IF(B17 &gt;  0,E17-B17, 0)</f>
-        <v>21</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="16" t="s">
-        <v>61</v>
+        <v>57</v>
+      </c>
+      <c r="B18" s="16">
+        <v>10110</v>
+      </c>
+      <c r="C18" s="16">
+        <v>10150</v>
+      </c>
+      <c r="D18" s="16">
+        <f t="shared" si="1"/>
+        <v>40</v>
       </c>
       <c r="E18">
-        <v>10254</v>
+        <v>10128</v>
+      </c>
+      <c r="F18" s="16">
+        <f>IF(B18 &gt;  0,E18-B18, 0)</f>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:6">
       <c r="A19" s="16" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B19" s="16">
-        <v>10733</v>
+        <v>10165</v>
       </c>
       <c r="C19" s="16">
-        <v>10777</v>
+        <v>10208</v>
       </c>
       <c r="D19" s="16">
         <f t="shared" si="1"/>
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E19">
-        <v>10746</v>
+        <v>10186</v>
       </c>
       <c r="F19" s="16">
         <f>IF(B19 &gt;  0,E19-B19, 0)</f>
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="A20" s="16" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E20">
-        <v>10769</v>
+        <v>10254</v>
       </c>
     </row>
     <row r="21" spans="1:6">
       <c r="A21" s="16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B21" s="16">
-        <v>11117</v>
+        <v>10733</v>
       </c>
       <c r="C21" s="16">
-        <v>11169</v>
+        <v>10777</v>
       </c>
       <c r="D21" s="16">
         <f t="shared" si="1"/>
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="E21">
-        <v>11144</v>
+        <v>10746</v>
       </c>
       <c r="F21" s="16">
         <f>IF(B21 &gt;  0,E21-B21, 0)</f>
-        <v>27</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:6">
       <c r="A22" s="16" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="16">
-        <v>11298</v>
-      </c>
-      <c r="C22" s="16">
-        <v>11349</v>
-      </c>
-      <c r="D22" s="16">
-        <f t="shared" si="1"/>
-        <v>51</v>
+        <v>63</v>
       </c>
       <c r="E22">
-        <v>11325</v>
-      </c>
-      <c r="F22" s="16">
-        <f>IF(B22 &gt;  0,E22-B22, 0)</f>
-        <v>27</v>
+        <v>10769</v>
       </c>
     </row>
     <row r="23" spans="1:6">
       <c r="A23" s="16" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B23" s="16">
-        <v>11439</v>
+        <v>11117</v>
       </c>
       <c r="C23" s="16">
-        <v>11490</v>
+        <v>11169</v>
       </c>
       <c r="D23" s="16">
         <f t="shared" si="1"/>
+        <v>52</v>
+      </c>
+      <c r="E23">
+        <v>11144</v>
+      </c>
+      <c r="F23" s="16">
+        <f t="shared" ref="F23:F28" si="2">IF(B23 &gt;  0,E23-B23, 0)</f>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="16">
+        <v>11298</v>
+      </c>
+      <c r="C24" s="16">
+        <v>11349</v>
+      </c>
+      <c r="D24" s="16">
+        <f t="shared" si="1"/>
         <v>51</v>
       </c>
-      <c r="E23">
-        <v>11466</v>
-      </c>
-      <c r="F23" s="16">
-        <f>IF(B23 &gt;  0,E23-B23, 0)</f>
+      <c r="E24">
+        <v>11325</v>
+      </c>
+      <c r="F24" s="16">
+        <f t="shared" si="2"/>
         <v>27</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="B24" s="16">
-        <v>11491</v>
-      </c>
-      <c r="C24" s="16">
-        <v>11542</v>
-      </c>
-      <c r="D24" s="16">
-        <f t="shared" si="1"/>
-        <v>51</v>
-      </c>
-      <c r="E24">
-        <v>11517</v>
-      </c>
-      <c r="F24" s="16">
-        <f>IF(B24 &gt;  0,E24-B24, 0)</f>
-        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:6">
       <c r="A25" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B25" s="16">
-        <v>11552</v>
+        <v>11439</v>
       </c>
       <c r="C25" s="16">
-        <v>11606</v>
+        <v>11490</v>
       </c>
       <c r="D25" s="16">
         <f t="shared" si="1"/>
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="E25">
-        <v>11577</v>
+        <v>11466</v>
       </c>
       <c r="F25" s="16">
-        <f>IF(B25 &gt;  0,E25-B25, 0)</f>
-        <v>25</v>
+        <f t="shared" si="2"/>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="16" t="s">
-        <v>69</v>
+      <c r="A26" s="18" t="s">
+        <v>67</v>
       </c>
       <c r="B26" s="16">
-        <v>11616</v>
+        <v>11491</v>
       </c>
       <c r="C26" s="16">
-        <v>11672</v>
+        <v>11542</v>
       </c>
       <c r="D26" s="16">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E26">
-        <v>11644</v>
+        <v>11517</v>
       </c>
       <c r="F26" s="16">
-        <f>IF(B26 &gt;  0,E26-B26, 0)</f>
-        <v>28</v>
+        <f t="shared" si="2"/>
+        <v>26</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="16" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B27" s="16">
-        <v>11626</v>
+        <v>11552</v>
       </c>
       <c r="C27" s="16">
-        <v>11682</v>
+        <v>11606</v>
       </c>
       <c r="D27" s="16">
         <f t="shared" si="1"/>
-        <v>56</v>
+        <v>54</v>
+      </c>
+      <c r="E27">
+        <v>11577</v>
+      </c>
+      <c r="F27" s="16">
+        <f t="shared" si="2"/>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:6">
       <c r="A28" s="16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B28" s="16">
-        <v>11652</v>
+        <v>11616</v>
       </c>
       <c r="C28" s="16">
-        <v>11708</v>
+        <v>11672</v>
       </c>
       <c r="D28" s="16">
         <f t="shared" si="1"/>
         <v>56</v>
       </c>
       <c r="E28">
-        <v>11680</v>
+        <v>11644</v>
       </c>
       <c r="F28" s="16">
-        <f>IF(B28 &gt;  0,E28-B28, 0)</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:6">
       <c r="A29" s="16" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B29" s="16">
-        <v>11810</v>
+        <v>11626</v>
       </c>
       <c r="C29" s="16">
-        <v>11870</v>
+        <v>11682</v>
       </c>
       <c r="D29" s="16">
         <f t="shared" si="1"/>
-        <v>60</v>
-      </c>
-      <c r="E29">
-        <v>11839</v>
-      </c>
-      <c r="F29" s="16">
-        <f>IF(B29 &gt;  0,E29-B29, 0)</f>
-        <v>29</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="18" t="s">
-        <v>45</v>
+      <c r="A30" s="16" t="s">
+        <v>71</v>
       </c>
       <c r="B30" s="16">
-        <v>12121</v>
+        <v>11652</v>
       </c>
       <c r="C30" s="16">
-        <v>12181</v>
+        <v>11708</v>
       </c>
       <c r="D30" s="16">
         <f t="shared" si="1"/>
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E30">
-        <v>12150</v>
+        <v>11680</v>
       </c>
       <c r="F30" s="16">
-        <f>IF(B30 &gt;  0,E30-B30, 0)</f>
-        <v>29</v>
+        <f t="shared" ref="F30:F36" si="3">IF(B30 &gt;  0,E30-B30, 0)</f>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:6">
       <c r="A31" s="16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="16">
-        <v>12635</v>
+        <v>11810</v>
       </c>
       <c r="C31" s="16">
-        <v>12695</v>
+        <v>11870</v>
       </c>
       <c r="D31" s="16">
         <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="E31">
-        <v>12664</v>
+        <v>11839</v>
       </c>
       <c r="F31" s="16">
-        <f>IF(B31 &gt;  0,E31-B31, 0)</f>
+        <f t="shared" si="3"/>
         <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="16" t="s">
-        <v>74</v>
+      <c r="A32" s="18" t="s">
+        <v>45</v>
       </c>
       <c r="B32" s="16">
-        <v>13099</v>
+        <v>12121</v>
       </c>
       <c r="C32" s="16">
-        <v>13187</v>
+        <v>12181</v>
       </c>
       <c r="D32" s="16">
         <f t="shared" si="1"/>
-        <v>88</v>
+        <v>60</v>
       </c>
       <c r="E32">
-        <v>13117</v>
+        <v>12150</v>
       </c>
       <c r="F32" s="16">
-        <f>IF(B32 &gt;  0,E32-B32, 0)</f>
-        <v>18</v>
+        <f t="shared" si="3"/>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:6">
       <c r="A33" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="16">
+        <v>12635</v>
+      </c>
+      <c r="C33" s="16">
+        <v>12695</v>
+      </c>
+      <c r="D33" s="16">
+        <f t="shared" si="1"/>
+        <v>60</v>
+      </c>
+      <c r="E33">
+        <v>12664</v>
+      </c>
+      <c r="F33" s="16">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B34" s="16">
+        <v>13099</v>
+      </c>
+      <c r="C34" s="16">
+        <v>13187</v>
+      </c>
+      <c r="D34" s="16">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="E34">
+        <v>13117</v>
+      </c>
+      <c r="F34" s="16">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="B33" s="16">
+      <c r="B35" s="16">
         <v>13343</v>
       </c>
-      <c r="C33" s="16">
+      <c r="C35" s="16">
         <v>13431</v>
       </c>
-      <c r="D33" s="16">
+      <c r="D35" s="16">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-      <c r="E33">
+      <c r="E35">
         <v>13361</v>
       </c>
-      <c r="F33" s="16">
-        <f>IF(B33 &gt;  0,E33-B33, 0)</f>
+      <c r="F35" s="16">
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
     </row>
+    <row r="36" spans="1:6">
+      <c r="A36" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="16">
+        <v>14307</v>
+      </c>
+      <c r="C36" s="16">
+        <v>14395</v>
+      </c>
+      <c r="D36" s="16">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+      <c r="E36">
+        <v>14325</v>
+      </c>
+      <c r="F36" s="16">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="18.75">
+      <c r="A37" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
+      <c r="D37" s="28"/>
+      <c r="E37" s="29"/>
+      <c r="F37" s="29"/>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="22"/>
+      <c r="C38" s="22"/>
+      <c r="D38" s="22"/>
+      <c r="E38" s="23"/>
+      <c r="F38" s="22"/>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39" s="16">
+        <v>15202</v>
+      </c>
+      <c r="C39" s="16">
+        <v>15292</v>
+      </c>
+      <c r="D39" s="16">
+        <f t="shared" ref="D39:D46" si="4">IF(B39 &gt;  0,C39-B39, 0)</f>
+        <v>90</v>
+      </c>
+      <c r="E39">
+        <v>15220</v>
+      </c>
+      <c r="F39" s="16">
+        <f t="shared" ref="F39:F46" si="5">IF(B39 &gt;  0,E39-B39, 0)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="16">
+        <v>16484</v>
+      </c>
+      <c r="C40" s="16">
+        <v>16574</v>
+      </c>
+      <c r="D40" s="16">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B41" s="16">
+        <v>17011</v>
+      </c>
+      <c r="C41" s="16">
+        <v>17101</v>
+      </c>
+      <c r="D41" s="16">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="E41">
+        <v>17027</v>
+      </c>
+      <c r="F41" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B42" s="16">
+        <v>17525</v>
+      </c>
+      <c r="C42" s="16">
+        <v>17615</v>
+      </c>
+      <c r="D42" s="16">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="E42">
+        <v>17541</v>
+      </c>
+      <c r="F42" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B43" s="16">
+        <v>18058</v>
+      </c>
+      <c r="C43" s="16">
+        <v>18298</v>
+      </c>
+      <c r="D43" s="16">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="E43">
+        <v>18074</v>
+      </c>
+      <c r="F43" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" s="22"/>
+      <c r="C44" s="22"/>
+      <c r="D44" s="22"/>
+      <c r="E44" s="23"/>
+      <c r="F44" s="22"/>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45" s="16">
+        <v>18356</v>
+      </c>
+      <c r="C45" s="16">
+        <v>18596</v>
+      </c>
+      <c r="D45" s="16">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="E45">
+        <v>18372</v>
+      </c>
+      <c r="F45" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="16">
+        <v>18742</v>
+      </c>
+      <c r="C46" s="16">
+        <v>18982</v>
+      </c>
+      <c r="D46" s="16">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="E46">
+        <v>18758</v>
+      </c>
+      <c r="F46" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A7:F7"/>
+    <mergeCell ref="A37:F37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>

<commit_message>
NSMB - a tad more progress, nothing significant though
</commit_message>
<xml_diff>
--- a/trunk/NSMB/NSMB.xlsx
+++ b/trunk/NSMB/NSMB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
   <si>
     <t>1-1</t>
   </si>
@@ -268,6 +268,12 @@
   </si>
   <si>
     <t>End Level</t>
+  </si>
+  <si>
+    <t>Checkpoint 10</t>
+  </si>
+  <si>
+    <t>Checkpoint 567</t>
   </si>
 </sst>
 </file>
@@ -722,11 +728,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A47" sqref="A47"/>
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1387,14 +1393,14 @@
         <v>15292</v>
       </c>
       <c r="D39" s="16">
-        <f t="shared" ref="D39:D46" si="4">IF(B39 &gt;  0,C39-B39, 0)</f>
+        <f t="shared" ref="D39:D48" si="4">IF(B39 &gt;  0,C39-B39, 0)</f>
         <v>90</v>
       </c>
       <c r="E39">
         <v>15220</v>
       </c>
       <c r="F39" s="16">
-        <f t="shared" ref="F39:F46" si="5">IF(B39 &gt;  0,E39-B39, 0)</f>
+        <f t="shared" ref="F39:F48" si="5">IF(B39 &gt;  0,E39-B39, 0)</f>
         <v>18</v>
       </c>
     </row>
@@ -1531,6 +1537,50 @@
       <c r="F46" s="16">
         <f t="shared" si="5"/>
         <v>16</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B47" s="16">
+        <v>18974</v>
+      </c>
+      <c r="C47" s="16">
+        <v>19214</v>
+      </c>
+      <c r="D47" s="16">
+        <f t="shared" si="4"/>
+        <v>240</v>
+      </c>
+      <c r="E47">
+        <v>18990</v>
+      </c>
+      <c r="F47" s="16">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
+      <c r="A48" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B48" s="16">
+        <v>19150</v>
+      </c>
+      <c r="C48" s="16">
+        <v>19392</v>
+      </c>
+      <c r="D48" s="16">
+        <f t="shared" si="4"/>
+        <v>242</v>
+      </c>
+      <c r="E48">
+        <v>19168</v>
+      </c>
+      <c r="F48" s="16">
+        <f t="shared" si="5"/>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - 5-2 done.  I saved just enough frames for a 367 final clock time! No need to slow down to 365, saved 48 frames.
</commit_message>
<xml_diff>
--- a/trunk/NSMB/NSMB.xlsx
+++ b/trunk/NSMB/NSMB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
   <si>
     <t>1-1</t>
   </si>
@@ -274,6 +274,30 @@
   </si>
   <si>
     <t>Checkpoint 567</t>
+  </si>
+  <si>
+    <t>Checkpoint 732</t>
+  </si>
+  <si>
+    <t>Checkpoint 949</t>
+  </si>
+  <si>
+    <t>Checkpoint 1154</t>
+  </si>
+  <si>
+    <t>Checkpoint 1221</t>
+  </si>
+  <si>
+    <t>Checkpoint 1470</t>
+  </si>
+  <si>
+    <t>Checkpoint 2208</t>
+  </si>
+  <si>
+    <t>Checkpoitn 3427 (1st time)</t>
+  </si>
+  <si>
+    <t>Checkpoint 3422 (2nd time)</t>
   </si>
 </sst>
 </file>
@@ -728,11 +752,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F48"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1393,14 +1417,14 @@
         <v>15292</v>
       </c>
       <c r="D39" s="16">
-        <f t="shared" ref="D39:D48" si="4">IF(B39 &gt;  0,C39-B39, 0)</f>
+        <f t="shared" ref="D39:D59" si="4">IF(B39 &gt;  0,C39-B39, 0)</f>
         <v>90</v>
       </c>
       <c r="E39">
         <v>15220</v>
       </c>
       <c r="F39" s="16">
-        <f t="shared" ref="F39:F48" si="5">IF(B39 &gt;  0,E39-B39, 0)</f>
+        <f t="shared" ref="F39:F50" si="5">IF(B39 &gt;  0,E39-B39, 0)</f>
         <v>18</v>
       </c>
     </row>
@@ -1566,21 +1590,200 @@
         <v>85</v>
       </c>
       <c r="B48" s="16">
-        <v>19150</v>
+        <v>19152</v>
       </c>
       <c r="C48" s="16">
         <v>19392</v>
       </c>
       <c r="D48" s="16">
         <f t="shared" si="4"/>
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="E48">
         <v>19168</v>
       </c>
       <c r="F48" s="16">
         <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B49" s="16">
+        <v>19206</v>
+      </c>
+      <c r="C49" s="16">
+        <v>19447</v>
+      </c>
+      <c r="D49" s="16">
+        <f t="shared" si="4"/>
+        <v>241</v>
+      </c>
+      <c r="E49">
+        <v>19223</v>
+      </c>
+      <c r="F49" s="16">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="16">
+        <v>19281</v>
+      </c>
+      <c r="C50" s="16">
+        <v>19522</v>
+      </c>
+      <c r="D50" s="16">
+        <f t="shared" si="4"/>
+        <v>241</v>
+      </c>
+      <c r="E50">
+        <v>19299</v>
+      </c>
+      <c r="F50" s="16">
+        <f t="shared" si="5"/>
         <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="16">
+        <v>19350</v>
+      </c>
+      <c r="C51" s="16">
+        <v>19591</v>
+      </c>
+      <c r="D51" s="16">
+        <f t="shared" si="4"/>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="B52" s="16">
+        <v>19374</v>
+      </c>
+      <c r="C52" s="16">
+        <v>19615</v>
+      </c>
+      <c r="D52" s="16">
+        <f t="shared" si="4"/>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="B53" s="16">
+        <v>19461</v>
+      </c>
+      <c r="C53" s="16">
+        <v>19703</v>
+      </c>
+      <c r="D53" s="16">
+        <f t="shared" si="4"/>
+        <v>242</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="16">
+        <v>19706</v>
+      </c>
+      <c r="C54" s="16">
+        <v>19949</v>
+      </c>
+      <c r="D54" s="16">
+        <f t="shared" si="4"/>
+        <v>243</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="16" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="16">
+        <v>20114</v>
+      </c>
+      <c r="C55" s="16">
+        <v>20359</v>
+      </c>
+      <c r="D55" s="16">
+        <f t="shared" si="4"/>
+        <v>245</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="16" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="16">
+        <v>20117</v>
+      </c>
+      <c r="C56" s="16">
+        <v>20363</v>
+      </c>
+      <c r="D56" s="16">
+        <f t="shared" si="4"/>
+        <v>246</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B57" s="16">
+        <v>20263</v>
+      </c>
+      <c r="C57" s="16">
+        <v>20512</v>
+      </c>
+      <c r="D57" s="16">
+        <f t="shared" si="4"/>
+        <v>249</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B58" s="16">
+        <v>20543</v>
+      </c>
+      <c r="C58" s="16">
+        <v>20832</v>
+      </c>
+      <c r="D58" s="16">
+        <f t="shared" si="4"/>
+        <v>289</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6">
+      <c r="A59" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B59" s="16">
+        <v>21058</v>
+      </c>
+      <c r="C59" s="16">
+        <v>21346</v>
+      </c>
+      <c r="D59" s="16">
+        <f t="shared" si="4"/>
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - 5-2 done 7 frames faster, still bad randomess with the map movements.  I don't know what to do to affect it.  Different frames, points, and coins haven't done anything.
</commit_message>
<xml_diff>
--- a/trunk/NSMB/NSMB.xlsx
+++ b/trunk/NSMB/NSMB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
   <si>
     <t>1-1</t>
   </si>
@@ -298,6 +298,12 @@
   </si>
   <si>
     <t>Checkpoint 3422 (2nd time)</t>
+  </si>
+  <si>
+    <t>Level 5-2</t>
+  </si>
+  <si>
+    <t>1st Move</t>
   </si>
 </sst>
 </file>
@@ -752,7 +758,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
@@ -1417,7 +1423,7 @@
         <v>15292</v>
       </c>
       <c r="D39" s="16">
-        <f t="shared" ref="D39:D59" si="4">IF(B39 &gt;  0,C39-B39, 0)</f>
+        <f t="shared" ref="D39:D60" si="4">IF(B39 &gt;  0,C39-B39, 0)</f>
         <v>90</v>
       </c>
       <c r="E39">
@@ -1511,7 +1517,7 @@
     </row>
     <row r="44" spans="1:6">
       <c r="A44" s="24" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="B44" s="22"/>
       <c r="C44" s="22"/>
@@ -1761,14 +1767,21 @@
         <v>45</v>
       </c>
       <c r="B58" s="16">
-        <v>20543</v>
+        <v>20537</v>
       </c>
       <c r="C58" s="16">
         <v>20832</v>
       </c>
       <c r="D58" s="16">
         <f t="shared" si="4"/>
-        <v>289</v>
+        <v>295</v>
+      </c>
+      <c r="E58">
+        <v>20600</v>
+      </c>
+      <c r="F58" s="16">
+        <f t="shared" ref="F58:F60" si="6">IF(B58 &gt;  0,E58-B58, 0)</f>
+        <v>63</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1776,14 +1789,43 @@
         <v>46</v>
       </c>
       <c r="B59" s="16">
-        <v>21058</v>
+        <v>21051</v>
       </c>
       <c r="C59" s="16">
         <v>21346</v>
       </c>
       <c r="D59" s="16">
         <f t="shared" si="4"/>
-        <v>288</v>
+        <v>295</v>
+      </c>
+      <c r="E59">
+        <v>21114</v>
+      </c>
+      <c r="F59" s="16">
+        <f t="shared" si="6"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B60" s="16">
+        <v>21617</v>
+      </c>
+      <c r="C60" s="16">
+        <v>22007</v>
+      </c>
+      <c r="D60" s="16">
+        <f t="shared" si="4"/>
+        <v>390</v>
+      </c>
+      <c r="E60">
+        <v>21615</v>
+      </c>
+      <c r="F60" s="16">
+        <f t="shared" si="6"/>
+        <v>-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
NSMB - this demonstrates my idea, getting mini-mario in 5-3.  It takes less backtracking in this level vs the Ghost house.  Also mini mario should be able to complete the level faster since he doesn't need to duck (shell) under the narrow paths.  Unfortunately the map manipulation isn't ideal and it costs potentially several hundred frames.
</commit_message>
<xml_diff>
--- a/trunk/NSMB/NSMB.xlsx
+++ b/trunk/NSMB/NSMB.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="99">
   <si>
     <t>1-1</t>
   </si>
@@ -304,6 +304,15 @@
   </si>
   <si>
     <t>1st Move</t>
+  </si>
+  <si>
+    <t>Score after bats: 97480</t>
+  </si>
+  <si>
+    <t>Tried: 97580 coin = 93</t>
+  </si>
+  <si>
+    <t>Tried: 97780 coin = 97</t>
   </si>
 </sst>
 </file>
@@ -758,11 +767,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F60"/>
+  <dimension ref="A1:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B60" sqref="B60"/>
+      <selection pane="bottomLeft" activeCell="E52" sqref="E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1613,7 +1622,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:6">
+    <row r="49" spans="1:7">
       <c r="A49" s="16" t="s">
         <v>86</v>
       </c>
@@ -1635,7 +1644,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:6">
+    <row r="50" spans="1:7">
       <c r="A50" s="16" t="s">
         <v>87</v>
       </c>
@@ -1657,7 +1666,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
+    <row r="51" spans="1:7">
       <c r="A51" s="16" t="s">
         <v>88</v>
       </c>
@@ -1672,7 +1681,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="52" spans="1:6">
+    <row r="52" spans="1:7">
       <c r="A52" s="16" t="s">
         <v>89</v>
       </c>
@@ -1687,7 +1696,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="53" spans="1:6">
+    <row r="53" spans="1:7">
       <c r="A53" s="16" t="s">
         <v>90</v>
       </c>
@@ -1702,7 +1711,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="54" spans="1:6">
+    <row r="54" spans="1:7">
       <c r="A54" s="16" t="s">
         <v>91</v>
       </c>
@@ -1717,7 +1726,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="55" spans="1:6">
+    <row r="55" spans="1:7">
       <c r="A55" s="16" t="s">
         <v>92</v>
       </c>
@@ -1732,7 +1741,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="56" spans="1:6">
+    <row r="56" spans="1:7">
       <c r="A56" s="16" t="s">
         <v>93</v>
       </c>
@@ -1747,22 +1756,22 @@
         <v>246</v>
       </c>
     </row>
-    <row r="57" spans="1:6">
+    <row r="57" spans="1:7">
       <c r="A57" s="16" t="s">
         <v>20</v>
       </c>
       <c r="B57" s="16">
-        <v>20263</v>
+        <v>20257</v>
       </c>
       <c r="C57" s="16">
         <v>20512</v>
       </c>
       <c r="D57" s="16">
         <f t="shared" si="4"/>
-        <v>249</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" s="16" t="s">
         <v>45</v>
       </c>
@@ -1783,8 +1792,11 @@
         <f t="shared" ref="F58:F60" si="6">IF(B58 &gt;  0,E58-B58, 0)</f>
         <v>63</v>
       </c>
-    </row>
-    <row r="59" spans="1:6">
+      <c r="G58" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" s="16" t="s">
         <v>46</v>
       </c>
@@ -1805,8 +1817,11 @@
         <f t="shared" si="6"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="60" spans="1:6">
+      <c r="G59" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" s="16" t="s">
         <v>95</v>
       </c>
@@ -1826,6 +1841,9 @@
       <c r="F60" s="16">
         <f t="shared" si="6"/>
         <v>-2</v>
+      </c>
+      <c r="G60" t="s">
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>